<commit_message>
update GSA_Sobol.jl and bounds.xlsx
</commit_message>
<xml_diff>
--- a/bounds.xlsx
+++ b/bounds.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\Billy\Documents\Math\Research\BGT_Sonographer\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28F40EC9-F5F9-4DF3-A178-46C47A053A8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3E44CD7-C358-477E-A6E0-B25872E89B3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="4500" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="mean" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="59">
   <si>
     <t>HC_min</t>
   </si>
@@ -200,12 +201,27 @@
   </si>
   <si>
     <t>BPD_max</t>
+  </si>
+  <si>
+    <t>BPD</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>AC</t>
+  </si>
+  <si>
+    <t>FL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -275,7 +291,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -294,11 +310,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="21">
+    <dxf>
+      <font>
+        <b/>
+        <charset val="161"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -430,7 +460,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A04E6302-28AD-49C2-88A7-EF4EC780A0EB}" name="Table1" displayName="Table1" ref="A1:I27" headerRowDxfId="19" dataDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A04E6302-28AD-49C2-88A7-EF4EC780A0EB}" name="Table1" displayName="Table1" ref="A1:I27" headerRowDxfId="20" dataDxfId="19">
   <autoFilter ref="A1:I27" xr:uid="{A04E6302-28AD-49C2-88A7-EF4EC780A0EB}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -443,17 +473,31 @@
     <filterColumn colId="8" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{C3B1D96D-B917-44C9-8958-78E344D2BB13}" name="week" totalsRowLabel="Total" dataDxfId="17" totalsRowDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{3E60AC80-E4CB-4330-8552-30A82CDF6248}" name="BPD_min" dataDxfId="15" totalsRowDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{AEB2FC05-6E55-4A40-BD1D-E265675021AA}" name="BPD_max" dataDxfId="13" totalsRowDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{1D387D25-014E-41C2-9359-F01765F69745}" name="HC_min" dataDxfId="11" totalsRowDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{90C8486E-D81D-4555-8DB3-A47843421043}" name="HC_max" dataDxfId="9" totalsRowDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{FC2DD16B-358F-403C-A343-90CEB3494DED}" name="AC_min" dataDxfId="7" totalsRowDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{34FF606D-9462-4551-B472-C67144ABA6CF}" name="AC_max" dataDxfId="5" totalsRowDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{F4990834-DB58-45EC-B8DF-0DAFBBB620F8}" name="FL_min" dataDxfId="3" totalsRowDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{D43D1070-0559-4079-BA9C-4BFA4C3722B5}" name="FL_max" totalsRowFunction="count" dataDxfId="1" totalsRowDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{C3B1D96D-B917-44C9-8958-78E344D2BB13}" name="week" totalsRowLabel="Total" dataDxfId="18" totalsRowDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{3E60AC80-E4CB-4330-8552-30A82CDF6248}" name="BPD_min" dataDxfId="16" totalsRowDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{AEB2FC05-6E55-4A40-BD1D-E265675021AA}" name="BPD_max" dataDxfId="14" totalsRowDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{1D387D25-014E-41C2-9359-F01765F69745}" name="HC_min" dataDxfId="12" totalsRowDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{90C8486E-D81D-4555-8DB3-A47843421043}" name="HC_max" dataDxfId="10" totalsRowDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{FC2DD16B-358F-403C-A343-90CEB3494DED}" name="AC_min" dataDxfId="8" totalsRowDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{34FF606D-9462-4551-B472-C67144ABA6CF}" name="AC_max" dataDxfId="6" totalsRowDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{F4990834-DB58-45EC-B8DF-0DAFBBB620F8}" name="FL_min" dataDxfId="4" totalsRowDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{D43D1070-0559-4079-BA9C-4BFA4C3722B5}" name="FL_max" totalsRowFunction="count" dataDxfId="2" totalsRowDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium17" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1309AEB8-D2E8-4812-98BB-6F7435C3B3B7}" name="Πίνακας1" displayName="Πίνακας1" ref="A1:E58" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:E58" xr:uid="{1309AEB8-D2E8-4812-98BB-6F7435C3B3B7}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{305ABA9C-B686-46D1-A414-2FF02E000DCD}" name="week"/>
+    <tableColumn id="2" xr3:uid="{F432AB4D-C921-49AE-948A-6471AE99818C}" name="BPD"/>
+    <tableColumn id="3" xr3:uid="{8B10CC49-1916-4325-9B89-60A1EBE7CE23}" name="HC"/>
+    <tableColumn id="4" xr3:uid="{CBBEDAAF-5E78-4F0A-B3B6-97BD2ACFA20E}" name="AC"/>
+    <tableColumn id="5" xr3:uid="{29FAB4D1-1110-49E6-A502-BCF58D4BCC6D}" name="FL"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -722,7 +766,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -1776,4 +1820,1008 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B427D037-D278-466E-921C-CC4259E2AB09}">
+  <dimension ref="A1:E58"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2">
+        <v>12</v>
+      </c>
+      <c r="B2">
+        <v>1.7</v>
+      </c>
+      <c r="C2">
+        <v>6.8</v>
+      </c>
+      <c r="D2">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E2">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>12.5</v>
+      </c>
+      <c r="B3">
+        <v>1.9</v>
+      </c>
+      <c r="C3">
+        <v>7.5</v>
+      </c>
+      <c r="D3">
+        <v>5.3</v>
+      </c>
+      <c r="E3">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <v>2.1</v>
+      </c>
+      <c r="C4">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="D4" s="10">
+        <v>6</v>
+      </c>
+      <c r="E4">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>13.5</v>
+      </c>
+      <c r="B5">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="C5">
+        <v>8.9</v>
+      </c>
+      <c r="D5">
+        <v>6.7</v>
+      </c>
+      <c r="E5">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>2.5</v>
+      </c>
+      <c r="C6">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="D6">
+        <v>7.3</v>
+      </c>
+      <c r="E6">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7">
+        <v>14.5</v>
+      </c>
+      <c r="B7">
+        <v>2.7</v>
+      </c>
+      <c r="C7">
+        <v>10.4</v>
+      </c>
+      <c r="D7" s="10">
+        <v>8</v>
+      </c>
+      <c r="E7">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <v>2.9</v>
+      </c>
+      <c r="C8" s="10">
+        <v>11</v>
+      </c>
+      <c r="D8">
+        <v>8.6</v>
+      </c>
+      <c r="E8">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9">
+        <v>15.5</v>
+      </c>
+      <c r="B9">
+        <v>3.1</v>
+      </c>
+      <c r="C9">
+        <v>11.7</v>
+      </c>
+      <c r="D9">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="E9">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10">
+        <v>16</v>
+      </c>
+      <c r="B10">
+        <v>3.2</v>
+      </c>
+      <c r="C10">
+        <v>12.4</v>
+      </c>
+      <c r="D10">
+        <v>9.9</v>
+      </c>
+      <c r="E10" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11">
+        <v>16.5</v>
+      </c>
+      <c r="B11">
+        <v>3.4</v>
+      </c>
+      <c r="C11">
+        <v>13.1</v>
+      </c>
+      <c r="D11">
+        <v>10.6</v>
+      </c>
+      <c r="E11">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12">
+        <v>17</v>
+      </c>
+      <c r="B12">
+        <v>3.6</v>
+      </c>
+      <c r="C12">
+        <v>13.8</v>
+      </c>
+      <c r="D12">
+        <v>11.2</v>
+      </c>
+      <c r="E12">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13">
+        <v>17.5</v>
+      </c>
+      <c r="B13">
+        <v>3.8</v>
+      </c>
+      <c r="C13">
+        <v>14.4</v>
+      </c>
+      <c r="D13">
+        <v>11.9</v>
+      </c>
+      <c r="E13">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14">
+        <v>18</v>
+      </c>
+      <c r="B14">
+        <v>3.9</v>
+      </c>
+      <c r="C14">
+        <v>15.1</v>
+      </c>
+      <c r="D14">
+        <v>12.5</v>
+      </c>
+      <c r="E14">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15">
+        <v>18.5</v>
+      </c>
+      <c r="B15">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C15">
+        <v>15.8</v>
+      </c>
+      <c r="D15">
+        <v>13.1</v>
+      </c>
+      <c r="E15">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16">
+        <v>19</v>
+      </c>
+      <c r="B16">
+        <v>4.3</v>
+      </c>
+      <c r="C16">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="D16">
+        <v>13.7</v>
+      </c>
+      <c r="E16" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17">
+        <v>19.5</v>
+      </c>
+      <c r="B17">
+        <v>4.5</v>
+      </c>
+      <c r="C17" s="10">
+        <v>17</v>
+      </c>
+      <c r="D17">
+        <v>14.4</v>
+      </c>
+      <c r="E17">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18">
+        <v>20</v>
+      </c>
+      <c r="B18">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="C18">
+        <v>17.7</v>
+      </c>
+      <c r="D18" s="10">
+        <v>15</v>
+      </c>
+      <c r="E18">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19">
+        <v>20.5</v>
+      </c>
+      <c r="B19">
+        <v>4.8</v>
+      </c>
+      <c r="C19">
+        <v>18.3</v>
+      </c>
+      <c r="D19">
+        <v>15.6</v>
+      </c>
+      <c r="E19">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20">
+        <v>21</v>
+      </c>
+      <c r="B20" s="10">
+        <v>5</v>
+      </c>
+      <c r="C20">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="D20">
+        <v>16.2</v>
+      </c>
+      <c r="E20">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21">
+        <v>21.5</v>
+      </c>
+      <c r="B21">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="C21">
+        <v>19.5</v>
+      </c>
+      <c r="D21">
+        <v>16.8</v>
+      </c>
+      <c r="E21">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22">
+        <v>22</v>
+      </c>
+      <c r="B22">
+        <v>5.3</v>
+      </c>
+      <c r="C22">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="D22">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="E22">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23">
+        <v>22.5</v>
+      </c>
+      <c r="B23">
+        <v>5.5</v>
+      </c>
+      <c r="C23">
+        <v>20.7</v>
+      </c>
+      <c r="D23">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="E23" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>5.6</v>
+      </c>
+      <c r="C24">
+        <v>21.3</v>
+      </c>
+      <c r="D24">
+        <v>18.5</v>
+      </c>
+      <c r="E24">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25">
+        <v>23.5</v>
+      </c>
+      <c r="B25">
+        <v>5.8</v>
+      </c>
+      <c r="C25">
+        <v>21.9</v>
+      </c>
+      <c r="D25">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="E25">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>5.9</v>
+      </c>
+      <c r="C26">
+        <v>22.4</v>
+      </c>
+      <c r="D26">
+        <v>19.7</v>
+      </c>
+      <c r="E26">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27">
+        <v>24.5</v>
+      </c>
+      <c r="B27">
+        <v>6.1</v>
+      </c>
+      <c r="C27" s="10">
+        <v>23</v>
+      </c>
+      <c r="D27">
+        <v>20.2</v>
+      </c>
+      <c r="E27">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28">
+        <v>25</v>
+      </c>
+      <c r="B28">
+        <v>6.2</v>
+      </c>
+      <c r="C28">
+        <v>23.5</v>
+      </c>
+      <c r="D28">
+        <v>20.8</v>
+      </c>
+      <c r="E28">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29">
+        <v>25.5</v>
+      </c>
+      <c r="B29">
+        <v>6.4</v>
+      </c>
+      <c r="C29">
+        <v>24.1</v>
+      </c>
+      <c r="D29">
+        <v>21.3</v>
+      </c>
+      <c r="E29">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30">
+        <v>26</v>
+      </c>
+      <c r="B30">
+        <v>6.5</v>
+      </c>
+      <c r="C30">
+        <v>24.6</v>
+      </c>
+      <c r="D30">
+        <v>21.9</v>
+      </c>
+      <c r="E30">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31">
+        <v>26.5</v>
+      </c>
+      <c r="B31">
+        <v>6.7</v>
+      </c>
+      <c r="C31">
+        <v>25.1</v>
+      </c>
+      <c r="D31">
+        <v>22.4</v>
+      </c>
+      <c r="E31" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32">
+        <v>27</v>
+      </c>
+      <c r="B32">
+        <v>6.8</v>
+      </c>
+      <c r="C32">
+        <v>25.6</v>
+      </c>
+      <c r="D32" s="10">
+        <v>23</v>
+      </c>
+      <c r="E32">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33">
+        <v>27.5</v>
+      </c>
+      <c r="B33">
+        <v>6.9</v>
+      </c>
+      <c r="C33">
+        <v>26.1</v>
+      </c>
+      <c r="D33">
+        <v>23.5</v>
+      </c>
+      <c r="E33">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34">
+        <v>28</v>
+      </c>
+      <c r="B34">
+        <v>7.1</v>
+      </c>
+      <c r="C34">
+        <v>26.6</v>
+      </c>
+      <c r="D34" s="10">
+        <v>24</v>
+      </c>
+      <c r="E34">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35">
+        <v>28.5</v>
+      </c>
+      <c r="B35">
+        <v>7.2</v>
+      </c>
+      <c r="C35">
+        <v>27.1</v>
+      </c>
+      <c r="D35">
+        <v>24.6</v>
+      </c>
+      <c r="E35">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36">
+        <v>29</v>
+      </c>
+      <c r="B36">
+        <v>7.3</v>
+      </c>
+      <c r="C36">
+        <v>27.5</v>
+      </c>
+      <c r="D36">
+        <v>25.1</v>
+      </c>
+      <c r="E36">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37">
+        <v>29.5</v>
+      </c>
+      <c r="B37">
+        <v>7.5</v>
+      </c>
+      <c r="C37" s="10">
+        <v>28</v>
+      </c>
+      <c r="D37">
+        <v>25.6</v>
+      </c>
+      <c r="E37">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38">
+        <v>30</v>
+      </c>
+      <c r="B38">
+        <v>7.6</v>
+      </c>
+      <c r="C38">
+        <v>28.4</v>
+      </c>
+      <c r="D38">
+        <v>26.1</v>
+      </c>
+      <c r="E38">
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39">
+        <v>30.5</v>
+      </c>
+      <c r="B39">
+        <v>7.7</v>
+      </c>
+      <c r="C39">
+        <v>28.8</v>
+      </c>
+      <c r="D39">
+        <v>26.6</v>
+      </c>
+      <c r="E39">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40">
+        <v>31</v>
+      </c>
+      <c r="B40">
+        <v>7.8</v>
+      </c>
+      <c r="C40">
+        <v>29.3</v>
+      </c>
+      <c r="D40">
+        <v>27.1</v>
+      </c>
+      <c r="E40" s="10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41">
+        <v>31.5</v>
+      </c>
+      <c r="B41">
+        <v>7.9</v>
+      </c>
+      <c r="C41">
+        <v>29.7</v>
+      </c>
+      <c r="D41">
+        <v>27.6</v>
+      </c>
+      <c r="E41">
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42">
+        <v>32</v>
+      </c>
+      <c r="B42">
+        <v>8.1</v>
+      </c>
+      <c r="C42">
+        <v>30.1</v>
+      </c>
+      <c r="D42">
+        <v>28.1</v>
+      </c>
+      <c r="E42">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43">
+        <v>32.5</v>
+      </c>
+      <c r="B43">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="C43">
+        <v>30.4</v>
+      </c>
+      <c r="D43">
+        <v>28.6</v>
+      </c>
+      <c r="E43">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44">
+        <v>33</v>
+      </c>
+      <c r="B44">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="C44">
+        <v>30.8</v>
+      </c>
+      <c r="D44">
+        <v>29.1</v>
+      </c>
+      <c r="E44">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45">
+        <v>33.5</v>
+      </c>
+      <c r="B45">
+        <v>8.4</v>
+      </c>
+      <c r="C45">
+        <v>31.2</v>
+      </c>
+      <c r="D45">
+        <v>29.5</v>
+      </c>
+      <c r="E45">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46">
+        <v>34</v>
+      </c>
+      <c r="B46">
+        <v>8.5</v>
+      </c>
+      <c r="C46">
+        <v>31.5</v>
+      </c>
+      <c r="D46" s="10">
+        <v>30</v>
+      </c>
+      <c r="E46">
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47">
+        <v>34.5</v>
+      </c>
+      <c r="B47">
+        <v>8.6</v>
+      </c>
+      <c r="C47">
+        <v>31.8</v>
+      </c>
+      <c r="D47">
+        <v>30.5</v>
+      </c>
+      <c r="E47">
+        <v>6.7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48">
+        <v>35</v>
+      </c>
+      <c r="B48">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="C48">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="D48">
+        <v>30.9</v>
+      </c>
+      <c r="E48">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49">
+        <v>35.5</v>
+      </c>
+      <c r="B49">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="C49">
+        <v>32.5</v>
+      </c>
+      <c r="D49">
+        <v>31.4</v>
+      </c>
+      <c r="E49">
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50">
+        <v>36</v>
+      </c>
+      <c r="B50">
+        <v>8.9</v>
+      </c>
+      <c r="C50">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="D50">
+        <v>31.8</v>
+      </c>
+      <c r="E50" s="10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51">
+        <v>36.5</v>
+      </c>
+      <c r="B51">
+        <v>8.9</v>
+      </c>
+      <c r="C51" s="10">
+        <v>33</v>
+      </c>
+      <c r="D51">
+        <v>32.299999999999997</v>
+      </c>
+      <c r="E51">
+        <v>7.1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52">
+        <v>37</v>
+      </c>
+      <c r="B52" s="10">
+        <v>9</v>
+      </c>
+      <c r="C52">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="D52">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="E52">
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53">
+        <v>37.5</v>
+      </c>
+      <c r="B53">
+        <v>9.1</v>
+      </c>
+      <c r="C53">
+        <v>33.5</v>
+      </c>
+      <c r="D53">
+        <v>33.200000000000003</v>
+      </c>
+      <c r="E53">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54">
+        <v>38</v>
+      </c>
+      <c r="B54">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="C54">
+        <v>33.799999999999997</v>
+      </c>
+      <c r="D54">
+        <v>33.6</v>
+      </c>
+      <c r="E54">
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55">
+        <v>38.5</v>
+      </c>
+      <c r="B55">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="C55" s="10">
+        <v>34</v>
+      </c>
+      <c r="D55" s="10">
+        <v>34</v>
+      </c>
+      <c r="E55">
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56">
+        <v>39</v>
+      </c>
+      <c r="B56">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="C56">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="D56">
+        <v>34.4</v>
+      </c>
+      <c r="E56">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57">
+        <v>39.5</v>
+      </c>
+      <c r="B57">
+        <v>9.4</v>
+      </c>
+      <c r="C57">
+        <v>34.4</v>
+      </c>
+      <c r="D57">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="E57">
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58">
+        <v>40</v>
+      </c>
+      <c r="B58">
+        <v>9.4</v>
+      </c>
+      <c r="C58">
+        <v>34.6</v>
+      </c>
+      <c r="D58">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="E58">
+        <v>7.7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>